<commit_message>
Ajout des dates formatés dans les auto evals
</commit_message>
<xml_diff>
--- a/DataFiles/Inputs_AutoEval.xlsx
+++ b/DataFiles/Inputs_AutoEval.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\09-P_Appro\PS-Eval\DataFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB228A65-F302-420C-8099-EA0831007815}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42025B80-8C32-4C8F-BC39-34B2E36B18EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{012834FC-60CF-404E-9E3E-302EA8078C17}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{012834FC-60CF-404E-9E3E-302EA8078C17}"/>
   </bookViews>
   <sheets>
     <sheet name="inputs" sheetId="3" r:id="rId1"/>
@@ -42,9 +42,6 @@
     <t>Enseignant</t>
   </si>
   <si>
-    <t>Date début</t>
-  </si>
-  <si>
     <t>Date fin</t>
   </si>
   <si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>Valeurs</t>
+  </si>
+  <si>
+    <t>Date debut</t>
   </si>
 </sst>
 </file>
@@ -132,8 +132,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,18 +451,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A680B354-E400-4890-989B-5DBD9C1F0966}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -469,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -477,28 +478,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1">
         <v>44949</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1">
         <v>45009</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>300</v>
@@ -506,7 +507,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7">
         <v>10</v>
@@ -514,15 +515,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -537,7 +538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15BBCFFD-9086-4D11-B5E2-D769F6D9E5FA}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -545,34 +546,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
         <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>